<commit_message>
Added PCB + Useful code commands
</commit_message>
<xml_diff>
--- a/Dingo Robot Bill of Materials.xlsx
+++ b/Dingo Robot Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/nfer0009_student_monash_edu/Documents/Uni Documents/FYP - Robot Quadruped/GITHUB/DingoQuadruped/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1537" documentId="13_ncr:1_{CAA3EA50-B21F-466C-8ACE-9AAFCB28345B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E8BC648-0717-4322-BC73-FB5745689C84}"/>
+  <xr:revisionPtr revIDLastSave="1540" documentId="13_ncr:1_{CAA3EA50-B21F-466C-8ACE-9AAFCB28345B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{735B8920-59E2-45E6-B14E-237D59D9DAD4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{22EC8EF3-3BC0-41AD-BD72-82C0B0212A30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22EC8EF3-3BC0-41AD-BD72-82C0B0212A30}"/>
   </bookViews>
   <sheets>
     <sheet name="Final BOM" sheetId="3" r:id="rId1"/>
@@ -1146,19 +1146,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1181,9 +1177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1235,19 +1228,10 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyBorder="1"/>
@@ -1288,23 +1272,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1312,15 +1286,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1339,12 +1304,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,6 +1319,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1399,7 +1359,64 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1731,1343 +1748,1343 @@
   </sheetPr>
   <dimension ref="A3:J71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.81640625" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" customWidth="1"/>
-    <col min="5" max="5" width="78.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="34.90625" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="78.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="15" thickBot="1"/>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:10" ht="30" customHeight="1" thickBot="1">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="21">
         <v>12</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="22">
         <f>500.29/12+33.58/12</f>
         <v>44.489166666666669</v>
       </c>
-      <c r="H5" s="43">
-        <f t="shared" ref="H5:H48" si="0">F5*G5</f>
+      <c r="H5" s="37">
+        <f>F5*G5</f>
         <v>533.87</v>
       </c>
-      <c r="J5" s="90"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1">
-      <c r="B6" s="77"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>127.9</v>
+      </c>
+      <c r="H6" s="7">
+        <f>F6*G6</f>
+        <v>127.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" customHeight="1">
+      <c r="B7" s="63"/>
+      <c r="C7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+      <c r="G7" s="22">
+        <v>64.66</v>
+      </c>
+      <c r="H7" s="7">
+        <f>F7*G7</f>
+        <v>64.66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15" customHeight="1">
+      <c r="B8" s="63"/>
+      <c r="C8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22">
+        <v>57.8</v>
+      </c>
+      <c r="H8" s="7">
+        <f>F8*G8</f>
+        <v>57.8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15" customHeight="1">
+      <c r="B9" s="63"/>
+      <c r="C9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="22">
+        <v>43.3</v>
+      </c>
+      <c r="H9" s="7">
+        <f>F9*G9</f>
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15" customHeight="1">
+      <c r="B10" s="63"/>
+      <c r="C10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22">
+        <v>21.42</v>
+      </c>
+      <c r="H10" s="7">
+        <f>F10*G10</f>
+        <v>42.84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15" customHeight="1">
+      <c r="B11" s="63"/>
+      <c r="C11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="22">
+        <v>30.06</v>
+      </c>
+      <c r="H11" s="7">
+        <f>F11*G11</f>
+        <v>30.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1">
+      <c r="B12" s="63"/>
+      <c r="C12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7">
+        <f>F12*G12</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" customHeight="1">
+      <c r="B13" s="63"/>
+      <c r="C13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>23.9</v>
+      </c>
+      <c r="H13" s="7">
+        <f>F13*G13</f>
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1">
+      <c r="B14" s="63"/>
+      <c r="C14" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" s="22">
+        <v>22.5</v>
+      </c>
+      <c r="H14" s="7">
+        <f>F14*G14</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" thickBot="1">
+      <c r="B15" s="64"/>
+      <c r="C15" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="47">
+        <v>1</v>
+      </c>
+      <c r="G15" s="56">
+        <v>20.57</v>
+      </c>
+      <c r="H15" s="41">
+        <f>F15*G15</f>
+        <v>20.57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B16" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13">
+        <v>19.95</v>
+      </c>
+      <c r="H16" s="49">
+        <f>F16*G16</f>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B17" s="63"/>
+      <c r="C17" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>19.75</v>
+      </c>
+      <c r="H17" s="7">
+        <f>F17*G17</f>
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B18" s="63"/>
+      <c r="C18" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6">
+        <v>19.27</v>
+      </c>
+      <c r="H18" s="7">
+        <f>F18*G18</f>
+        <v>19.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B19" s="63"/>
+      <c r="C19" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>19</v>
+      </c>
+      <c r="H19" s="9">
+        <f>F19*G19</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.45" customHeight="1">
+      <c r="B20" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4</v>
+      </c>
+      <c r="G20" s="22">
+        <v>4.57</v>
+      </c>
+      <c r="H20" s="37">
+        <f>F20*G20</f>
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.45" customHeight="1">
+      <c r="B21" s="63"/>
+      <c r="C21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>12.49</v>
+      </c>
+      <c r="H21" s="7">
+        <f>F21*G21</f>
+        <v>12.49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.45" customHeight="1">
+      <c r="B22" s="63"/>
+      <c r="C22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6">
+        <v>11.29</v>
+      </c>
+      <c r="H22" s="7">
+        <f>F22*G22</f>
+        <v>11.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.45" customHeight="1">
+      <c r="B23" s="63"/>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4</v>
+      </c>
+      <c r="G23" s="6">
+        <v>2.36</v>
+      </c>
+      <c r="H23" s="7">
+        <f>F23*G23</f>
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.45" customHeight="1" thickBot="1">
+      <c r="B24" s="63"/>
+      <c r="C24" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" s="92">
+        <v>1</v>
+      </c>
+      <c r="G24" s="95">
+        <v>8.9</v>
+      </c>
+      <c r="H24" s="7">
+        <f>F24*G24</f>
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="B25" s="63"/>
+      <c r="C25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="26">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H25" s="7">
+        <f>F25*G25</f>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B26" s="64"/>
+      <c r="C26" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="25">
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <v>7.99</v>
+      </c>
+      <c r="H26" s="41">
+        <f>F26*G26</f>
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A27" s="43"/>
+      <c r="B27" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="88">
+        <v>1935776</v>
+      </c>
+      <c r="F27" s="91">
+        <v>8</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.92</v>
+      </c>
+      <c r="H27" s="49">
+        <f>F27*G27</f>
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="A28" s="43"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D28" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E28" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F28" s="25">
         <v>4</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G28" s="6">
         <v>1.77</v>
       </c>
-      <c r="H6" s="9">
-        <f t="shared" si="0"/>
+      <c r="H28" s="41">
+        <f>F28*G28</f>
         <v>7.08</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" customHeight="1">
-      <c r="B7" s="77"/>
-      <c r="C7" s="21" t="s">
+    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="A29" s="43"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="25">
+        <v>1</v>
+      </c>
+      <c r="G29" s="26">
+        <v>6.95</v>
+      </c>
+      <c r="H29" s="41">
+        <f>F29*G29</f>
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.45" customHeight="1" thickBot="1">
+      <c r="A30" s="43"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8">
+        <v>6.54</v>
+      </c>
+      <c r="H30" s="9">
+        <f>F30*G30</f>
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A31" s="43"/>
+      <c r="B31" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="21">
+        <v>8</v>
+      </c>
+      <c r="G31" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="H31" s="37">
+        <f>F31*G31</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A32" s="43"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32" s="30">
+        <v>5.19</v>
+      </c>
+      <c r="H32" s="7">
+        <f>F32*G32</f>
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A33" s="43"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
+        <v>5.19</v>
+      </c>
+      <c r="H33" s="7">
+        <f>F33*G33</f>
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A34" s="43"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H34" s="7">
+        <f>F34*G34</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A35" s="43"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="H35" s="7">
+        <f>F35*G35</f>
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A36" s="43"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="30">
+        <v>3.25</v>
+      </c>
+      <c r="H36" s="7">
+        <f>F36*G36</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A37" s="43"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>2.76</v>
+      </c>
+      <c r="H37" s="7">
+        <f>F37*G37</f>
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" thickBot="1">
+      <c r="A38" s="43"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="25">
+        <v>1</v>
+      </c>
+      <c r="G38" s="26">
+        <v>2.6</v>
+      </c>
+      <c r="H38" s="41">
+        <f>F38*G38</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="91">
         <v>12</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="24">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25">
-        <v>12.49</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="0"/>
-        <v>12.49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="15" customHeight="1">
-      <c r="B8" s="77"/>
-      <c r="C8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="24">
-        <v>1</v>
-      </c>
-      <c r="G8" s="25">
-        <v>11.29</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="shared" si="0"/>
-        <v>11.29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15" customHeight="1">
-      <c r="B9" s="77"/>
-      <c r="C9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="24">
-        <v>4</v>
-      </c>
-      <c r="G9" s="25">
-        <v>4.57</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>18.28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15" customHeight="1">
-      <c r="B10" s="77"/>
-      <c r="C10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="24">
-        <v>4</v>
-      </c>
-      <c r="G10" s="25">
-        <v>2.36</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>9.44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1">
-      <c r="B11" s="77"/>
-      <c r="C11" s="21" t="s">
+      <c r="G39" s="13">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="H39" s="49">
+        <f>F39*G39</f>
+        <v>2.544</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" s="63"/>
+      <c r="C40" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="H40" s="7">
+        <f>F40*G40</f>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" s="63"/>
+      <c r="C41" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="29">
+        <v>25</v>
+      </c>
+      <c r="G41" s="6">
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="H41" s="7">
+        <f>F41*G41</f>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" s="63"/>
+      <c r="C42" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D42" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E42" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="24">
-        <v>1</v>
-      </c>
-      <c r="G11" s="25">
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6">
         <v>1.26</v>
       </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
+      <c r="H42" s="7">
+        <f>F42*G42</f>
         <v>1.26</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1">
-      <c r="B12" s="77"/>
-      <c r="C12" s="21" t="s">
+    <row r="43" spans="1:8">
+      <c r="B43" s="63"/>
+      <c r="C43" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="29">
+        <v>12</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="H43" s="7">
+        <f>F43*G43</f>
+        <v>1.236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="63"/>
+      <c r="C44" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H44" s="7">
+        <f>F44*G44</f>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45" s="63"/>
+      <c r="C45" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D45" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="24">
-        <v>1</v>
-      </c>
-      <c r="G12" s="25">
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H12" s="9">
-        <f t="shared" si="0"/>
+      <c r="H45" s="7">
+        <f>F45*G45</f>
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1">
-      <c r="B13" s="77"/>
-      <c r="C13" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" s="24">
-        <v>1</v>
-      </c>
-      <c r="G13" s="25">
-        <v>5.19</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>5.19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1">
-      <c r="B14" s="77"/>
-      <c r="C14" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="24">
-        <v>1</v>
-      </c>
-      <c r="G14" s="25">
-        <v>5.19</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="0"/>
-        <v>5.19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="78"/>
-      <c r="C15" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" s="56">
-        <v>1</v>
-      </c>
-      <c r="G15" s="69">
-        <v>6.54</v>
-      </c>
-      <c r="H15" s="47">
-        <f t="shared" si="0"/>
-        <v>6.54</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B16" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="70" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="15">
-        <v>1</v>
-      </c>
-      <c r="G16" s="16">
-        <v>2.6</v>
-      </c>
-      <c r="H16" s="59">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B17" s="77"/>
-      <c r="C17" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8">
-        <v>4.8099999999999996</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="shared" si="0"/>
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B18" s="77"/>
-      <c r="C18" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="7">
-        <v>8</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="H18" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B19" s="77"/>
-      <c r="C19" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="12">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10">
-        <v>22.5</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="0"/>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.5" customHeight="1">
-      <c r="B20" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="24">
-        <v>1</v>
-      </c>
-      <c r="G20" s="25">
-        <v>23.9</v>
-      </c>
-      <c r="H20" s="43">
-        <f t="shared" si="0"/>
-        <v>23.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.5" customHeight="1">
-      <c r="B21" s="77"/>
-      <c r="C21" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="8">
-        <v>127.9</v>
-      </c>
-      <c r="H21" s="9">
-        <f t="shared" si="0"/>
-        <v>127.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14.5" customHeight="1">
-      <c r="B22" s="77"/>
-      <c r="C22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="7">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="H22" s="9">
-        <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="14.5" customHeight="1">
-      <c r="B23" s="77"/>
-      <c r="C23" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" s="7">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8">
-        <v>43.3</v>
-      </c>
-      <c r="H23" s="9">
-        <f t="shared" si="0"/>
-        <v>43.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="14.5" customHeight="1" thickBot="1">
-      <c r="B24" s="77"/>
-      <c r="C24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="7">
-        <v>1</v>
-      </c>
-      <c r="G24" s="8">
-        <v>7.99</v>
-      </c>
-      <c r="H24" s="9">
-        <f t="shared" si="0"/>
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="B25" s="77"/>
-      <c r="C25" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1</v>
-      </c>
-      <c r="G25" s="29">
-        <v>6.95</v>
-      </c>
-      <c r="H25" s="9">
-        <f t="shared" si="0"/>
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B26" s="78"/>
-      <c r="C26" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="28">
-        <v>1</v>
-      </c>
-      <c r="G26" s="29">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="H26" s="47">
-        <f t="shared" si="0"/>
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="77" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="15">
-        <v>1</v>
-      </c>
-      <c r="G27" s="16">
-        <v>20.57</v>
-      </c>
-      <c r="H27" s="59">
-        <f t="shared" si="0"/>
-        <v>20.57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="8">
-        <v>64.66</v>
-      </c>
-      <c r="H28" s="47">
-        <f t="shared" si="0"/>
-        <v>64.66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="49"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="60" t="s">
-        <v>172</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" s="28">
-        <v>1</v>
-      </c>
-      <c r="G29" s="29">
-        <v>19.75</v>
-      </c>
-      <c r="H29" s="47">
-        <f t="shared" si="0"/>
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="14.5" customHeight="1" thickBot="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="F30" s="53">
-        <v>1</v>
-      </c>
-      <c r="G30" s="54">
-        <v>8.9</v>
-      </c>
-      <c r="H30" s="11">
-        <f t="shared" si="0"/>
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A31" s="49"/>
-      <c r="B31" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="24">
-        <v>1</v>
-      </c>
-      <c r="G31" s="25">
-        <v>30</v>
-      </c>
-      <c r="H31" s="43">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A32" s="49"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="13" t="s">
+    <row r="46" spans="1:8">
+      <c r="B46" s="63"/>
+      <c r="C46" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D46" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E46" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="33">
-        <v>1</v>
-      </c>
-      <c r="G32" s="35">
+      <c r="F46" s="29">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
         <v>0.35</v>
       </c>
-      <c r="H32" s="9">
-        <f t="shared" si="0"/>
+      <c r="H46" s="7">
+        <f>F46*G46</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A33" s="49"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="36">
-        <v>1935776</v>
-      </c>
-      <c r="F33" s="33">
-        <v>8</v>
-      </c>
-      <c r="G33" s="8">
-        <v>0.92</v>
-      </c>
-      <c r="H33" s="9">
-        <f t="shared" si="0"/>
-        <v>7.36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="33">
-        <v>12</v>
-      </c>
-      <c r="G34" s="8">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="H34" s="9">
-        <f t="shared" si="0"/>
-        <v>2.544</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A35" s="49"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="33">
-        <v>12</v>
-      </c>
-      <c r="G35" s="8">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="H35" s="9">
-        <f t="shared" si="0"/>
-        <v>1.236</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A36" s="49"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="33">
-        <v>25</v>
-      </c>
-      <c r="G36" s="35">
-        <v>5.3600000000000002E-2</v>
-      </c>
-      <c r="H36" s="9">
-        <f t="shared" si="0"/>
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A37" s="49"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="13" t="s">
+    <row r="47" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B47" s="64"/>
+      <c r="C47" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D47" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E47" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="33">
-        <v>1</v>
-      </c>
-      <c r="G37" s="8">
+      <c r="F47" s="94">
+        <v>1</v>
+      </c>
+      <c r="G47" s="8">
         <v>0.16</v>
       </c>
-      <c r="H37" s="9">
-        <f t="shared" si="0"/>
+      <c r="H47" s="9">
+        <f>F47*G47</f>
         <v>0.16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A38" s="49"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="60" t="s">
+    <row r="48" spans="1:8">
+      <c r="B48" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="61" t="s">
+      <c r="D48" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="62" t="s">
+      <c r="E48" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="63">
-        <v>1</v>
-      </c>
-      <c r="G38" s="29">
+      <c r="F48" s="93">
+        <v>1</v>
+      </c>
+      <c r="G48" s="22">
         <v>0.16</v>
       </c>
-      <c r="H38" s="47">
-        <f t="shared" si="0"/>
+      <c r="H48" s="37">
+        <f>F48*G48</f>
         <v>0.16</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="B39" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="64" t="s">
+    <row r="49" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B49" s="64"/>
+      <c r="C49" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="8">
         <v>79</v>
       </c>
-      <c r="D39" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="15">
-        <v>1</v>
-      </c>
-      <c r="G39" s="16">
-        <v>19.27</v>
-      </c>
-      <c r="H39" s="59">
-        <f t="shared" si="0"/>
-        <v>19.27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="B40" s="77"/>
-      <c r="C40" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" s="7">
-        <v>1</v>
-      </c>
-      <c r="G40" s="8">
-        <v>2.76</v>
-      </c>
-      <c r="H40" s="9">
-        <f t="shared" si="0"/>
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="B41" s="77"/>
-      <c r="C41" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="8">
-        <v>19.95</v>
-      </c>
-      <c r="H41" s="9">
-        <f t="shared" si="0"/>
-        <v>19.95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="B42" s="77"/>
-      <c r="C42" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1</v>
-      </c>
-      <c r="G42" s="8">
-        <v>3.25</v>
-      </c>
-      <c r="H42" s="9">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="B43" s="77"/>
-      <c r="C43" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="7">
-        <v>1</v>
-      </c>
-      <c r="G43" s="8">
-        <v>30.06</v>
-      </c>
-      <c r="H43" s="9">
-        <f t="shared" si="0"/>
-        <v>30.06</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="B44" s="77"/>
-      <c r="C44" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F44" s="7">
-        <v>1</v>
-      </c>
-      <c r="G44" s="8">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H44" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="B45" s="77"/>
-      <c r="C45" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" s="7">
-        <v>2</v>
-      </c>
-      <c r="G45" s="8">
-        <v>21.42</v>
-      </c>
-      <c r="H45" s="9">
-        <f t="shared" si="0"/>
-        <v>42.84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="B46" s="77"/>
-      <c r="C46" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="7">
-        <v>1</v>
-      </c>
-      <c r="G46" s="8">
-        <v>57.8</v>
-      </c>
-      <c r="H46" s="9">
-        <f t="shared" si="0"/>
-        <v>57.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1">
-      <c r="B47" s="78"/>
-      <c r="C47" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F47" s="12">
-        <v>1</v>
-      </c>
-      <c r="G47" s="10">
-        <v>1.73</v>
-      </c>
-      <c r="H47" s="11">
-        <f t="shared" si="0"/>
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="B48" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="24">
-        <v>1</v>
-      </c>
-      <c r="G48" s="25">
-        <v>19</v>
-      </c>
-      <c r="H48" s="43">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="15" thickBot="1">
-      <c r="B49" s="78"/>
-      <c r="C49" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="D49" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" s="12">
-        <v>1</v>
-      </c>
-      <c r="G49" s="10">
-        <v>79</v>
-      </c>
-      <c r="H49" s="11">
+      <c r="H49" s="9">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="36.65" customHeight="1">
-      <c r="B50" s="79" t="s">
+    <row r="50" spans="2:8" ht="36.6" customHeight="1">
+      <c r="B50" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="81"/>
-    </row>
-    <row r="51" spans="2:8" ht="34.25" customHeight="1" thickBot="1">
-      <c r="B51" s="82"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="84"/>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="85" t="s">
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
+    </row>
+    <row r="51" spans="2:8" ht="34.35" customHeight="1" thickBot="1">
+      <c r="B51" s="68"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="70"/>
+    </row>
+    <row r="52" spans="2:8" ht="30">
+      <c r="B52" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D52" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F52" s="15">
+      <c r="F52" s="12">
         <v>2E-3</v>
       </c>
-      <c r="G52" s="16">
+      <c r="G52" s="13">
         <v>187.29</v>
       </c>
-      <c r="H52" s="59">
-        <f t="shared" ref="H52:H62" si="1">F52*G52</f>
+      <c r="H52" s="49">
+        <f t="shared" ref="H52:H62" si="0">F52*G52</f>
         <v>0.37457999999999997</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="14.5" customHeight="1">
-      <c r="B53" s="86"/>
-      <c r="C53" s="13" t="s">
+    <row r="53" spans="2:8" ht="14.45" customHeight="1">
+      <c r="B53" s="72"/>
+      <c r="C53" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="5">
         <v>0.05</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="6">
         <v>7.95</v>
       </c>
-      <c r="H53" s="9">
-        <f t="shared" si="1"/>
+      <c r="H53" s="7">
+        <f t="shared" si="0"/>
         <v>0.39750000000000002</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="14.5" customHeight="1">
-      <c r="B54" s="86"/>
-      <c r="C54" s="13" t="s">
+    <row r="54" spans="2:8" ht="14.45" customHeight="1">
+      <c r="B54" s="72"/>
+      <c r="C54" s="11" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="5">
         <v>20</v>
       </c>
-      <c r="G54" s="40">
+      <c r="G54" s="34">
         <v>0.24199999999999999</v>
       </c>
-      <c r="H54" s="9">
-        <f t="shared" si="1"/>
+      <c r="H54" s="7">
+        <f t="shared" si="0"/>
         <v>4.84</v>
       </c>
     </row>
     <row r="55" spans="2:8">
-      <c r="B55" s="86"/>
-      <c r="C55" s="13" t="s">
+      <c r="B55" s="72"/>
+      <c r="C55" s="11" t="s">
         <v>116</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E55" s="39" t="s">
+      <c r="E55" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="5">
         <v>0.1</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="6">
         <v>3</v>
       </c>
-      <c r="H55" s="9">
-        <f t="shared" si="1"/>
+      <c r="H55" s="7">
+        <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="15" thickBot="1">
-      <c r="B56" s="87"/>
-      <c r="C56" s="48" t="s">
+    <row r="56" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B56" s="73"/>
+      <c r="C56" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="45" t="s">
+      <c r="D56" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F56" s="12">
+      <c r="F56" s="10">
         <v>2</v>
       </c>
-      <c r="G56" s="10">
+      <c r="G56" s="8">
         <v>0.75</v>
       </c>
-      <c r="H56" s="11">
-        <f t="shared" si="1"/>
+      <c r="H56" s="9">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="57" spans="2:8">
-      <c r="B57" s="88" t="s">
+      <c r="B57" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E57" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="F57" s="24">
-        <v>1</v>
-      </c>
-      <c r="G57" s="25">
+      <c r="F57" s="21">
+        <v>1</v>
+      </c>
+      <c r="G57" s="22">
         <v>1.74</v>
       </c>
-      <c r="H57" s="43">
-        <f t="shared" si="1"/>
+      <c r="H57" s="37">
+        <f t="shared" si="0"/>
         <v>1.74</v>
       </c>
     </row>
     <row r="58" spans="2:8">
-      <c r="B58" s="88"/>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="74"/>
+      <c r="C58" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="E58" s="23" t="s">
+      <c r="E58" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="F58" s="24">
-        <v>1</v>
-      </c>
-      <c r="G58" s="25">
+      <c r="F58" s="21">
+        <v>1</v>
+      </c>
+      <c r="G58" s="22">
         <v>9.67</v>
       </c>
-      <c r="H58" s="9">
-        <f t="shared" si="1"/>
+      <c r="H58" s="7">
+        <f t="shared" si="0"/>
         <v>9.67</v>
       </c>
     </row>
     <row r="59" spans="2:8">
-      <c r="B59" s="88"/>
-      <c r="C59" s="38" t="s">
+      <c r="B59" s="74"/>
+      <c r="C59" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="23" t="s">
+      <c r="E59" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F59" s="24">
+      <c r="F59" s="21">
         <v>0.5</v>
       </c>
-      <c r="G59" s="25">
+      <c r="G59" s="22">
         <v>24.95</v>
       </c>
-      <c r="H59" s="9">
-        <f t="shared" si="1"/>
+      <c r="H59" s="7">
+        <f t="shared" si="0"/>
         <v>12.475</v>
       </c>
     </row>
     <row r="60" spans="2:8">
-      <c r="B60" s="88"/>
-      <c r="C60" s="38" t="s">
+      <c r="B60" s="74"/>
+      <c r="C60" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="23" t="s">
+      <c r="E60" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F60" s="24">
+      <c r="F60" s="21">
         <v>0.5</v>
       </c>
-      <c r="G60" s="25">
+      <c r="G60" s="22">
         <v>24.95</v>
       </c>
-      <c r="H60" s="9">
-        <f t="shared" si="1"/>
+      <c r="H60" s="7">
+        <f t="shared" si="0"/>
         <v>12.475</v>
       </c>
     </row>
     <row r="61" spans="2:8">
-      <c r="B61" s="88"/>
-      <c r="C61" s="38" t="s">
+      <c r="B61" s="74"/>
+      <c r="C61" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D61" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="23" t="s">
+      <c r="E61" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F61" s="24">
+      <c r="F61" s="21">
         <v>0.75</v>
       </c>
-      <c r="G61" s="25">
+      <c r="G61" s="22">
         <v>25.95</v>
       </c>
-      <c r="H61" s="9">
-        <f t="shared" si="1"/>
+      <c r="H61" s="7">
+        <f t="shared" si="0"/>
         <v>19.462499999999999</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="15" thickBot="1">
-      <c r="B62" s="89"/>
-      <c r="C62" s="44" t="s">
+    <row r="62" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B62" s="75"/>
+      <c r="C62" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="45" t="s">
+      <c r="D62" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="E62" s="42" t="s">
+      <c r="E62" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="F62" s="12">
+      <c r="F62" s="10">
         <v>0.05</v>
       </c>
-      <c r="G62" s="10">
+      <c r="G62" s="8">
         <v>33.950000000000003</v>
       </c>
-      <c r="H62" s="11">
-        <f t="shared" si="1"/>
+      <c r="H62" s="9">
+        <f t="shared" si="0"/>
         <v>1.6975000000000002</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="15" thickBot="1"/>
-    <row r="65" spans="5:10" ht="15" thickBot="1">
-      <c r="G65" s="76" t="s">
+    <row r="64" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="65" spans="5:10" ht="15.75" thickBot="1">
+      <c r="G65" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="H65" s="19">
+      <c r="H65" s="16">
         <f>SUM(H5:H63)</f>
         <v>1290.69208</v>
       </c>
     </row>
     <row r="66" spans="5:10">
-      <c r="J66" s="55"/>
+      <c r="J66" s="46"/>
     </row>
     <row r="71" spans="5:10">
       <c r="E71" t="s">
@@ -3075,6 +3092,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H49">
+    <sortCondition descending="1" ref="H5:H49"/>
+  </sortState>
   <mergeCells count="10">
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="B50:H51"/>
@@ -3094,25 +3114,25 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{141604F2-87C5-44E6-B708-9C8D8CBCA280}"/>
-    <hyperlink ref="D41" r:id="rId2" xr:uid="{7D523BC3-9906-44F3-A020-C711A6E4976F}"/>
-    <hyperlink ref="D30" r:id="rId3" xr:uid="{620C1AEE-96AD-4323-A512-A5E5C898EFA9}"/>
-    <hyperlink ref="D27" r:id="rId4" xr:uid="{69137084-0139-4C20-8C98-4B29826EDD6A}"/>
-    <hyperlink ref="D39" r:id="rId5" xr:uid="{06FD3702-EEE9-438D-8C68-0E89E4A59868}"/>
-    <hyperlink ref="D40" r:id="rId6" xr:uid="{A7D78203-1ACD-4914-BF4A-49D1DC856A90}"/>
-    <hyperlink ref="E46" r:id="rId7" display="https://core-electronics.com.au/speaker-pcb-mount.html " xr:uid="{02AD4126-755C-4B8D-8E4E-FB5C019DD0DF}"/>
-    <hyperlink ref="D18" r:id="rId8" display="https://magnet.com.au/products/neodymium-disc-6mm-x-2mm-diametric-n35?variant=37006186971301&amp;currency=AUD&amp;utm_source=google&amp;utm_medium=&amp;utm_id=17632686716&amp;utm_content=&amp;utm_term=&amp;creativeId=&amp;gclid=CjwKCAjwwL6aBhBlEiwADycBIIdzTlagejPUPeQ-sVTDDbsELvUR1bW7tAAXokLwELk8-JGPUlBU4RoCnNMQAvD_BwE&amp;_atid=yoAZS1xoT68WGERHBMpsSoIidnjEej&amp;fbclid=IwAR1iOjxi2imSJXPCzrt-8cT2lWh2TofaApdKMH6VuEt5qIHqTee9IJKkoPo" xr:uid="{2DD39543-FB2B-43D7-AAE2-71336E49F3E1}"/>
-    <hyperlink ref="D26" r:id="rId9" xr:uid="{B531CCB2-887E-495E-9E25-AC554C1CE074}"/>
-    <hyperlink ref="D48" r:id="rId10" xr:uid="{2D0FAD7A-7F58-43C1-A182-B7965742B4A3}"/>
-    <hyperlink ref="D20" r:id="rId11" xr:uid="{E399CC72-84E0-4346-B715-CD7EA6759C15}"/>
-    <hyperlink ref="D33" r:id="rId12" xr:uid="{A7FAB41A-23BF-469E-BB4D-E97461D0E59B}"/>
-    <hyperlink ref="D38" r:id="rId13" xr:uid="{17E457E6-BA96-42B1-9A7C-4163706ED7B9}"/>
-    <hyperlink ref="D37" r:id="rId14" xr:uid="{A30DA4D4-AB0C-4863-8358-08EF5767F970}"/>
-    <hyperlink ref="D34" r:id="rId15" xr:uid="{AE9E74EE-4A30-4D83-8A84-4CDAA9500030}"/>
-    <hyperlink ref="D32" r:id="rId16" xr:uid="{1DED6DD8-949F-492C-92AE-08AC4950B1E8}"/>
-    <hyperlink ref="D36" r:id="rId17" xr:uid="{5C26A4C3-94BB-47B7-8AA7-D2B533396047}"/>
-    <hyperlink ref="D35" r:id="rId18" xr:uid="{94FA71A8-7A21-42C8-B87F-00323B5C7F29}"/>
-    <hyperlink ref="D7" r:id="rId19" xr:uid="{1BB8D0BC-0728-460B-B589-0B0F351F6157}"/>
-    <hyperlink ref="D23" r:id="rId20" xr:uid="{9CD28BD0-CCFF-4FCA-B0DA-F75C41B3FFB9}"/>
+    <hyperlink ref="D16" r:id="rId2" xr:uid="{7D523BC3-9906-44F3-A020-C711A6E4976F}"/>
+    <hyperlink ref="D24" r:id="rId3" xr:uid="{620C1AEE-96AD-4323-A512-A5E5C898EFA9}"/>
+    <hyperlink ref="D15" r:id="rId4" xr:uid="{69137084-0139-4C20-8C98-4B29826EDD6A}"/>
+    <hyperlink ref="D18" r:id="rId5" xr:uid="{06FD3702-EEE9-438D-8C68-0E89E4A59868}"/>
+    <hyperlink ref="D37" r:id="rId6" xr:uid="{A7D78203-1ACD-4914-BF4A-49D1DC856A90}"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://core-electronics.com.au/speaker-pcb-mount.html " xr:uid="{02AD4126-755C-4B8D-8E4E-FB5C019DD0DF}"/>
+    <hyperlink ref="D31" r:id="rId8" display="https://magnet.com.au/products/neodymium-disc-6mm-x-2mm-diametric-n35?variant=37006186971301&amp;currency=AUD&amp;utm_source=google&amp;utm_medium=&amp;utm_id=17632686716&amp;utm_content=&amp;utm_term=&amp;creativeId=&amp;gclid=CjwKCAjwwL6aBhBlEiwADycBIIdzTlagejPUPeQ-sVTDDbsELvUR1bW7tAAXokLwELk8-JGPUlBU4RoCnNMQAvD_BwE&amp;_atid=yoAZS1xoT68WGERHBMpsSoIidnjEej&amp;fbclid=IwAR1iOjxi2imSJXPCzrt-8cT2lWh2TofaApdKMH6VuEt5qIHqTee9IJKkoPo" xr:uid="{2DD39543-FB2B-43D7-AAE2-71336E49F3E1}"/>
+    <hyperlink ref="D25" r:id="rId9" xr:uid="{B531CCB2-887E-495E-9E25-AC554C1CE074}"/>
+    <hyperlink ref="D19" r:id="rId10" xr:uid="{2D0FAD7A-7F58-43C1-A182-B7965742B4A3}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{E399CC72-84E0-4346-B715-CD7EA6759C15}"/>
+    <hyperlink ref="D27" r:id="rId12" xr:uid="{A7FAB41A-23BF-469E-BB4D-E97461D0E59B}"/>
+    <hyperlink ref="D48" r:id="rId13" xr:uid="{17E457E6-BA96-42B1-9A7C-4163706ED7B9}"/>
+    <hyperlink ref="D47" r:id="rId14" xr:uid="{A30DA4D4-AB0C-4863-8358-08EF5767F970}"/>
+    <hyperlink ref="D39" r:id="rId15" xr:uid="{AE9E74EE-4A30-4D83-8A84-4CDAA9500030}"/>
+    <hyperlink ref="D46" r:id="rId16" xr:uid="{1DED6DD8-949F-492C-92AE-08AC4950B1E8}"/>
+    <hyperlink ref="D41" r:id="rId17" xr:uid="{5C26A4C3-94BB-47B7-8AA7-D2B533396047}"/>
+    <hyperlink ref="D43" r:id="rId18" xr:uid="{94FA71A8-7A21-42C8-B87F-00323B5C7F29}"/>
+    <hyperlink ref="D21" r:id="rId19" xr:uid="{1BB8D0BC-0728-460B-B589-0B0F351F6157}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{9CD28BD0-CCFF-4FCA-B0DA-F75C41B3FFB9}"/>
     <hyperlink ref="D44" r:id="rId21" xr:uid="{068FC64E-8EC2-4D40-AADA-A93BBD3E5903}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3132,6 +3152,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8CA98ECE203BB4B925C834CEB10A6AE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="060b792a624e77254af64989d38d3799">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8aa7eb64-6cd0-4ccd-96dc-30da49f87ba6" xmlns:ns3="116b0b0f-b750-4427-bbba-efc7c0159ae8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2206fdaff9b63786624c091a2672d49a" ns2:_="" ns3:_="">
     <xsd:import namespace="8aa7eb64-6cd0-4ccd-96dc-30da49f87ba6"/>
@@ -3354,15 +3383,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F912A9B-F116-4526-B841-C5C66B9C094C}">
   <ds:schemaRefs>
@@ -3375,6 +3395,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B61558F-6849-4DF0-BD8F-6C563A5483A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{491227EF-0A20-4848-A3E5-7DBEFE81A4FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3391,12 +3419,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B61558F-6849-4DF0-BD8F-6C563A5483A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>